<commit_message>
WIP: translating rolling window to python
</commit_message>
<xml_diff>
--- a/data/analysis.xlsx
+++ b/data/analysis.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd6cb69810148686/Área de Trabalho/BDAQ/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd6cb69810148686/Área de Trabalho/python/BDAQ/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="167" documentId="11_AD4D361C20488DEA4E38A0CAEC1D76C45BDEDD81" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0B1BBC1-1B78-482A-8998-B2AAA2AFA2C3}"/>
+  <xr:revisionPtr revIDLastSave="183" documentId="11_AD4D361C20488DEA4E38A0CAEC1D76C45BDEDD81" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCA930E8-6A9A-4B0D-9B57-76C9804000F6}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$I$2:$J$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Plan1!$I$2:$J$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$J$3:$K$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Plan1!$J$3:$K$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="31">
   <si>
     <t>Portfolio</t>
   </si>
@@ -125,6 +125,15 @@
   </si>
   <si>
     <t>Resultado do impeachment Dilma</t>
+  </si>
+  <si>
+    <t>*resultado do brexit</t>
+  </si>
+  <si>
+    <t>*invasão do capitólio</t>
+  </si>
+  <si>
+    <t>*Início da guerra na ucrânia</t>
   </si>
 </sst>
 </file>
@@ -134,7 +143,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="0.0000%"/>
+    <numFmt numFmtId="165" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -280,7 +289,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -289,36 +298,34 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,650 +607,660 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="B2:K27"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="59.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="1.140625" customWidth="1"/>
+    <col min="10" max="10" width="59.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="7" t="s">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="17"/>
+      <c r="C3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5">
-        <v>17.057843944150999</v>
-      </c>
-      <c r="D2" s="5">
-        <v>24.79784337026619</v>
-      </c>
-      <c r="E2" s="5">
-        <v>0.68545654113341925</v>
-      </c>
-      <c r="F2" s="5">
-        <v>1.038158542003278</v>
-      </c>
-      <c r="G2" s="5">
-        <v>7.1627402919907128</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="D3" s="5">
+        <v>17.66844471405463</v>
+      </c>
+      <c r="E3" s="5">
+        <v>23.730703173750161</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.74201108096671564</v>
+      </c>
+      <c r="G3" s="5">
+        <v>1.305573997661102</v>
+      </c>
+      <c r="H3" s="5">
+        <v>6.9922092178877033</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="7" t="s">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="17"/>
+      <c r="C4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5">
-        <v>13.837582032845701</v>
-      </c>
-      <c r="D3" s="5">
-        <v>19.585100996035639</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0.70347260581574445</v>
-      </c>
-      <c r="F3" s="5">
-        <v>0.97755551983819444</v>
-      </c>
-      <c r="G3" s="5">
-        <v>5.6723517599398861</v>
-      </c>
-      <c r="I3" s="21" t="s">
+      <c r="D4" s="5">
+        <v>14.735419841880031</v>
+      </c>
+      <c r="E4" s="5">
+        <v>18.65086695561742</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.7868492052837236</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1.209939020860741</v>
+      </c>
+      <c r="H4" s="5">
+        <v>5.4956825527022941</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="20">
+      <c r="K4" s="11">
         <v>39708</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="7" t="s">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="17"/>
+      <c r="C5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5">
-        <v>11.9385429361517</v>
-      </c>
-      <c r="D4" s="5">
-        <v>17.66760453147625</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0.67233466285647647</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0.96579583891965604</v>
-      </c>
-      <c r="G4" s="5">
-        <v>5.0872348095671898</v>
-      </c>
-      <c r="I4" s="21" t="s">
+      <c r="D5" s="5">
+        <v>13.052918616467069</v>
+      </c>
+      <c r="E5" s="5">
+        <v>17.09425770168847</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.76007504059001696</v>
+      </c>
+      <c r="G5" s="5">
+        <v>1.1694493362317031</v>
+      </c>
+      <c r="H5" s="5">
+        <v>5.022278589382549</v>
+      </c>
+      <c r="J5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="20">
+      <c r="K5" s="11">
         <v>41715</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+    <row r="6" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="J6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="20">
+      <c r="K6" s="11">
         <v>42174</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="7" t="s">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="19"/>
+      <c r="C7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="6">
+      <c r="D7" s="6">
         <v>17.801554435094669</v>
       </c>
-      <c r="D6" s="6">
+      <c r="E7" s="6">
         <v>24.737015291858601</v>
       </c>
-      <c r="E6" s="6">
+      <c r="F7" s="6">
         <v>0.71720675375633236</v>
       </c>
-      <c r="F6" s="6">
+      <c r="G7" s="6">
         <v>1.0840858493332279</v>
       </c>
-      <c r="G6" s="6">
+      <c r="H7" s="6">
         <v>7.0691393222567491</v>
       </c>
-      <c r="I6" s="21" t="s">
+      <c r="J7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="20">
+      <c r="K7" s="11">
         <v>42613</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="7" t="s">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="19"/>
+      <c r="C8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6">
+      <c r="D8" s="6">
         <v>14.491593635312629</v>
       </c>
-      <c r="D7" s="6">
+      <c r="E8" s="6">
         <v>19.472711086134439</v>
       </c>
-      <c r="E7" s="6">
+      <c r="F8" s="6">
         <v>0.74111886996508958</v>
       </c>
-      <c r="F7" s="6">
+      <c r="G8" s="6">
         <v>1.027975409989373</v>
       </c>
-      <c r="G7" s="6">
+      <c r="H8" s="6">
         <v>5.591157159241984</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="J8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="20">
+      <c r="K8" s="11">
         <v>42872</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="7" t="s">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="19"/>
+      <c r="C9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="6">
+      <c r="D9" s="6">
         <v>12.557575656130579</v>
       </c>
-      <c r="D8" s="6">
+      <c r="E9" s="6">
         <v>17.566522367197528</v>
       </c>
-      <c r="E8" s="6">
+      <c r="F9" s="6">
         <v>0.71144278844102127</v>
       </c>
-      <c r="F8" s="6">
+      <c r="G9" s="6">
         <v>1.0197887810932531</v>
       </c>
-      <c r="G8" s="6">
+      <c r="H9" s="6">
         <v>5.0308222692473326</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="J9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="20">
+      <c r="K9" s="11">
         <v>43241</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="10" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="J10" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="20">
+      <c r="K10" s="11">
         <v>43402</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="7" t="s">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="17"/>
+      <c r="C11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="8">
-        <v>13.756322599167291</v>
-      </c>
-      <c r="D10" s="6">
-        <v>25.294912482200431</v>
-      </c>
-      <c r="E10" s="6">
-        <v>0.54146550650472269</v>
-      </c>
-      <c r="F10" s="6">
-        <v>0.81177200937056904</v>
-      </c>
-      <c r="G10" s="6">
-        <v>7.3003977100006372</v>
-      </c>
-      <c r="I10" s="21" t="s">
+      <c r="D11" s="6">
+        <v>13.90949261935522</v>
+      </c>
+      <c r="E11" s="6">
+        <v>23.842572517127731</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0.58087241254718558</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1.0701260191248569</v>
+      </c>
+      <c r="H11" s="6">
+        <v>7.0771603818323152</v>
+      </c>
+      <c r="J11" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J10" s="20">
+      <c r="K11" s="11">
         <v>43830</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="7" t="s">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="17"/>
+      <c r="C12" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="6">
-        <v>11.307218795282539</v>
-      </c>
-      <c r="D11" s="6">
-        <v>19.73510093743376</v>
-      </c>
-      <c r="E11" s="6">
-        <v>0.56990936255860147</v>
-      </c>
-      <c r="F11" s="6">
-        <v>0.81539014899167428</v>
-      </c>
-      <c r="G11" s="6">
-        <v>5.9527716929260297</v>
-      </c>
-      <c r="I11" s="21" t="s">
+      <c r="D12" s="6">
+        <v>12.474921093453361</v>
+      </c>
+      <c r="E12" s="6">
+        <v>18.270462718253039</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0.67950775439585775</v>
+      </c>
+      <c r="G12" s="6">
+        <v>1.1748261619186751</v>
+      </c>
+      <c r="H12" s="6">
+        <v>5.7470764046951288</v>
+      </c>
+      <c r="J12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="20">
+      <c r="K12" s="11">
         <v>43887</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="7" t="s">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="17"/>
+      <c r="C13" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="6">
-        <v>9.9362414694875305</v>
-      </c>
-      <c r="D12" s="6">
-        <v>15.86145919357411</v>
-      </c>
-      <c r="E12" s="6">
-        <v>0.62265655063366754</v>
-      </c>
-      <c r="F12" s="6">
-        <v>0.89947366733273215</v>
-      </c>
-      <c r="G12" s="6">
-        <v>5.0180376909435722</v>
-      </c>
-      <c r="I12" s="21" t="s">
+      <c r="D13" s="6">
+        <v>11.13331018869496</v>
+      </c>
+      <c r="E13" s="6">
+        <v>14.2105713162964</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0.77923047161350312</v>
+      </c>
+      <c r="G13" s="6">
+        <v>1.36681778862738</v>
+      </c>
+      <c r="H13" s="6">
+        <v>4.8209848548668486</v>
+      </c>
+      <c r="J13" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="20">
+      <c r="K13" s="11">
         <v>43941</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+    <row r="14" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="7" t="s">
+      <c r="J14" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="19"/>
+      <c r="C15" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="6">
+      <c r="D15" s="6">
         <v>14.715214898855431</v>
       </c>
-      <c r="D14" s="6">
+      <c r="E15" s="6">
         <v>25.23498026605721</v>
       </c>
-      <c r="E14" s="6">
+      <c r="F15" s="6">
         <v>0.58075000433298174</v>
       </c>
-      <c r="F14" s="6">
+      <c r="G15" s="6">
         <v>0.86903238849637598</v>
       </c>
-      <c r="G14" s="6">
+      <c r="H15" s="6">
         <v>7.1718627505287538</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="7" t="s">
+      <c r="J15" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="19"/>
+      <c r="C16" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="6">
+      <c r="D16" s="6">
         <v>12.34708097561643</v>
       </c>
-      <c r="D15" s="6">
+      <c r="E16" s="6">
         <v>19.64771690439941</v>
       </c>
-      <c r="E15" s="6">
+      <c r="F16" s="6">
         <v>0.62536940222633031</v>
       </c>
-      <c r="F15" s="6">
+      <c r="G16" s="6">
         <v>0.89426775589831431</v>
       </c>
-      <c r="G15" s="6">
+      <c r="H16" s="6">
         <v>5.8711398168250479</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="7" t="s">
+      <c r="J16" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="19"/>
+      <c r="C17" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="6">
+      <c r="D17" s="6">
         <v>10.83257239056803</v>
       </c>
-      <c r="D16" s="6">
+      <c r="E17" s="6">
         <v>15.80260535824584</v>
       </c>
-      <c r="E16" s="6">
+      <c r="F17" s="6">
         <v>0.68169597014880001</v>
       </c>
-      <c r="F16" s="6">
+      <c r="G17" s="6">
         <v>0.9831246926594257</v>
       </c>
-      <c r="G16" s="6">
+      <c r="H17" s="6">
         <v>4.9959569692168548</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="13" t="s">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C19" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="7" t="s">
+    <row r="21" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="13"/>
+      <c r="C21" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="18">
-        <f>C2/C6-1</f>
-        <v>-4.1777839887818469E-2</v>
-      </c>
-      <c r="D20" s="18">
-        <f t="shared" ref="D20:G20" si="0">D2/D6-1</f>
-        <v>2.458990209203149E-3</v>
-      </c>
-      <c r="E20" s="18">
+      <c r="D21" s="9">
+        <f>D3/D7-1</f>
+        <v>-7.4774212288799546E-3</v>
+      </c>
+      <c r="E21" s="9">
+        <f t="shared" ref="E21:H21" si="0">E3/E7-1</f>
+        <v>-4.0680417836812977E-2</v>
+      </c>
+      <c r="F21" s="9">
         <f t="shared" si="0"/>
-        <v>-4.4269260511871966E-2</v>
-      </c>
-      <c r="F20" s="18">
+        <v>3.4584625814623182E-2</v>
+      </c>
+      <c r="G21" s="9">
         <f t="shared" si="0"/>
-        <v>-4.2365009522260411E-2</v>
-      </c>
-      <c r="G20" s="18">
+        <v>0.20430867948705478</v>
+      </c>
+      <c r="H21" s="9">
         <f t="shared" si="0"/>
-        <v>1.3240787239723328E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="7" t="s">
+        <v>-1.0882527682943843E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="13"/>
+      <c r="C22" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="18">
-        <f t="shared" ref="C21:G21" si="1">C3/C7-1</f>
-        <v>-4.51304127707014E-2</v>
-      </c>
-      <c r="D21" s="18">
+      <c r="D22" s="9">
+        <f t="shared" ref="D22:H22" si="1">D4/D8-1</f>
+        <v>1.6825354940484649E-2</v>
+      </c>
+      <c r="E22" s="9">
         <f t="shared" si="1"/>
-        <v>5.771662168871261E-3</v>
-      </c>
-      <c r="E21" s="18">
+        <v>-4.220491573472851E-2</v>
+      </c>
+      <c r="F22" s="9">
         <f t="shared" si="1"/>
-        <v>-5.0796526272659182E-2</v>
-      </c>
-      <c r="F21" s="18">
+        <v>6.1704454132692765E-2</v>
+      </c>
+      <c r="G22" s="9">
         <f t="shared" si="1"/>
-        <v>-4.9047758984526402E-2</v>
-      </c>
-      <c r="G21" s="18">
+        <v>0.17701163773289985</v>
+      </c>
+      <c r="H22" s="9">
         <f t="shared" si="1"/>
-        <v>1.4521967168046768E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="7" t="s">
+        <v>-1.7076001232030125E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="13"/>
+      <c r="C23" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="18">
-        <f t="shared" ref="C22:G22" si="2">C4/C8-1</f>
-        <v>-4.9295559662956845E-2</v>
-      </c>
-      <c r="D22" s="18">
+      <c r="D23" s="9">
+        <f t="shared" ref="D23:H23" si="2">D5/D9-1</f>
+        <v>3.9445747642751883E-2</v>
+      </c>
+      <c r="E23" s="9">
         <f t="shared" si="2"/>
-        <v>5.7542501677780855E-3</v>
-      </c>
-      <c r="E22" s="18">
+        <v>-2.6884357395117187E-2</v>
+      </c>
+      <c r="F23" s="9">
         <f t="shared" si="2"/>
-        <v>-5.4970162351693941E-2</v>
-      </c>
-      <c r="F22" s="18">
+        <v>6.8357221324237605E-2</v>
+      </c>
+      <c r="G23" s="9">
         <f t="shared" si="2"/>
-        <v>-5.2945220789460512E-2</v>
-      </c>
-      <c r="G22" s="18">
+        <v>0.14675642438231962</v>
+      </c>
+      <c r="H23" s="9">
         <f t="shared" si="2"/>
-        <v>1.1213383677793232E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
+        <v>-1.6982670838939784E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="D24" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="E24" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="F24" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F23" s="19" t="s">
+      <c r="G24" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="H24" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="7" t="s">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="15"/>
+      <c r="C25" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="18">
-        <f t="shared" ref="C24:G24" si="3">C6/C10-1</f>
-        <v>0.29406346112966619</v>
-      </c>
-      <c r="D24" s="18">
+      <c r="D25" s="9">
+        <f>D11/D15-1</f>
+        <v>-5.4754367166114593E-2</v>
+      </c>
+      <c r="E25" s="9">
+        <f t="shared" ref="E25:H25" si="3">E11/E15-1</f>
+        <v>-5.5177683289190593E-2</v>
+      </c>
+      <c r="F25" s="9">
         <f t="shared" si="3"/>
-        <v>-2.2055707476134279E-2</v>
-      </c>
-      <c r="E24" s="18">
+        <v>2.1077608831787664E-4</v>
+      </c>
+      <c r="G25" s="9">
         <f t="shared" si="3"/>
-        <v>0.32456591443111038</v>
-      </c>
-      <c r="F24" s="18">
+        <v>0.23139946599276784</v>
+      </c>
+      <c r="H25" s="9">
         <f t="shared" si="3"/>
-        <v>0.33545606009968898</v>
-      </c>
-      <c r="G24" s="18">
-        <f t="shared" si="3"/>
-        <v>-3.1677505381260684E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="7" t="s">
+        <v>-1.3204710127707964E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="15"/>
+      <c r="C26" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="18">
-        <f t="shared" ref="C25:G25" si="4">C7/C11-1</f>
-        <v>0.2816231734508079</v>
-      </c>
-      <c r="D25" s="18">
+      <c r="D26" s="9">
+        <f t="shared" ref="D26:H26" si="4">D12/D16-1</f>
+        <v>1.0353873768981892E-2</v>
+      </c>
+      <c r="E26" s="9">
         <f t="shared" si="4"/>
-        <v>-1.3295592058595318E-2</v>
-      </c>
-      <c r="E25" s="18">
+        <v>-7.0097416043183314E-2</v>
+      </c>
+      <c r="F26" s="9">
         <f t="shared" si="4"/>
-        <v>0.3004153268123988</v>
-      </c>
-      <c r="F25" s="18">
+        <v>8.6570196713803949E-2</v>
+      </c>
+      <c r="G26" s="9">
         <f t="shared" si="4"/>
-        <v>0.26071600357275027</v>
-      </c>
-      <c r="G25" s="18">
+        <v>0.31372975730130492</v>
+      </c>
+      <c r="H26" s="9">
         <f t="shared" si="4"/>
-        <v>-6.0747253941180079E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="7" t="s">
+        <v>-2.1131060748100006E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="15"/>
+      <c r="C27" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="18">
-        <f t="shared" ref="C26:G26" si="5">C8/C12-1</f>
-        <v>0.26381546731656136</v>
-      </c>
-      <c r="D26" s="18">
+      <c r="D27" s="9">
+        <f t="shared" ref="D27:H27" si="5">D13/D17-1</f>
+        <v>2.7762362187284673E-2</v>
+      </c>
+      <c r="E27" s="9">
         <f t="shared" si="5"/>
-        <v>0.10749724554435591</v>
-      </c>
-      <c r="E26" s="18">
+        <v>-0.10074503576201199</v>
+      </c>
+      <c r="F27" s="9">
         <f t="shared" si="5"/>
-        <v>0.14259263428128621</v>
-      </c>
-      <c r="F26" s="18">
+        <v>0.14307624767594462</v>
+      </c>
+      <c r="G27" s="9">
         <f t="shared" si="5"/>
-        <v>0.1337616854502246</v>
-      </c>
-      <c r="G26" s="18">
+        <v>0.39027917702894421</v>
+      </c>
+      <c r="H27" s="9">
         <f t="shared" si="5"/>
-        <v>2.5477246467944248E-3</v>
+        <v>-3.5022742475188773E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1254,8 +1271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1055BD-0D6A-4E2C-9ED2-852FB6ADF423}">
   <dimension ref="K2:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:L5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,70 +1306,70 @@
       </c>
     </row>
     <row r="3" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="20">
+      <c r="L3" s="11">
         <v>39708</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O3" s="20">
+      <c r="O3" s="11">
         <v>42613</v>
       </c>
-      <c r="Q3" s="21" t="s">
+      <c r="Q3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="R3" s="20">
+      <c r="R3" s="11">
         <v>43402</v>
       </c>
     </row>
     <row r="4" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K4" s="21" t="s">
+      <c r="K4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="20">
+      <c r="L4" s="11">
         <v>41715</v>
       </c>
-      <c r="N4" s="21" t="s">
+      <c r="N4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="20">
+      <c r="O4" s="11">
         <v>42872</v>
       </c>
-      <c r="Q4" s="21" t="s">
+      <c r="Q4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="R4" s="20">
+      <c r="R4" s="11">
         <v>43830</v>
       </c>
     </row>
     <row r="5" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K5" s="21" t="s">
+      <c r="K5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="20">
+      <c r="L5" s="11">
         <v>42174</v>
       </c>
-      <c r="N5" s="21" t="s">
+      <c r="N5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="20">
+      <c r="O5" s="11">
         <v>43241</v>
       </c>
-      <c r="Q5" s="21" t="s">
+      <c r="Q5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="R5" s="20">
+      <c r="R5" s="11">
         <v>43887</v>
       </c>
     </row>
     <row r="6" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="Q6" s="21" t="s">
+      <c r="Q6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="R6" s="20">
+      <c r="R6" s="11">
         <v>43941</v>
       </c>
     </row>

</xml_diff>